<commit_message>
Database scheme added + pdf file
</commit_message>
<xml_diff>
--- a/MySql/DatabaseScheme.xlsx
+++ b/MySql/DatabaseScheme.xlsx
@@ -245,49 +245,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
       <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal style="none"/>
     </border>
     <border>
@@ -305,130 +268,27 @@
       </bottom>
       <diagonal style="none"/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="1" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +798,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -976,657 +840,624 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="M4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="T5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="V5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J6">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <v>0</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="K6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" s="12" t="b">
+      <c r="O6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="V6" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" ht="14.25"/>
     <row r="10" ht="14.25">
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="11" t="s">
+      <c r="P11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U11" s="7" t="s">
+      <c r="U11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V11" s="7" t="s">
+      <c r="V11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="7" t="s">
+      <c r="W11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X11" s="7" t="s">
+      <c r="X11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="7">
         <v>0</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="7">
         <v>0</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="S12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="W12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="X12" s="13" t="b">
+      <c r="Q12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="V12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="13" t="b">
+      <c r="Q13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="R13" s="13" t="b">
+      <c r="R13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="S13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="V13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="W13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="X13" s="13" t="b">
+      <c r="S13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="V13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X13" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="16"/>
-    </row>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="17" ht="14.25"/>
     <row r="18" ht="14.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="F18" s="4" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="19"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="19"/>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="M20" s="20"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="22"/>
-    </row>
+    </row>
+    <row r="20" ht="14.25"/>
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25"/>
     <row r="23" ht="14.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M24" s="7" t="s">
+      <c r="M24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="7" t="s">
+      <c r="N24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="O24" s="7" t="s">
+      <c r="O24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M29" s="7" t="s">
+      <c r="M29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="7" t="s">
+      <c r="N29" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="42" ht="14.25"/>
     <row r="43" ht="14.25">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
     </row>
     <row r="44" ht="14.25">
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="47" ht="14.25"/>
     <row r="48" ht="14.25">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B4:K4"/>
     <mergeCell ref="M4:V4"/>
     <mergeCell ref="M10:X10"/>
     <mergeCell ref="B13:E13"/>
@@ -1641,7 +1472,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="36" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SQL Scheme file added
</commit_message>
<xml_diff>
--- a/MySql/DatabaseScheme.xlsx
+++ b/MySql/DatabaseScheme.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>users</t>
   </si>
   <si>
-    <t>global_premissions</t>
+    <t>global_permissions</t>
   </si>
   <si>
     <t>id_user</t>
@@ -87,7 +87,7 @@
     <t>admin</t>
   </si>
   <si>
-    <t>group_premissions</t>
+    <t>group_permissions</t>
   </si>
   <si>
     <t>id_group_premission</t>
@@ -96,7 +96,7 @@
     <t>id_group</t>
   </si>
   <si>
-    <t>group_permission</t>
+    <t>group_user_permission</t>
   </si>
   <si>
     <t>Creator</t>
@@ -126,10 +126,10 @@
     <t>id_task</t>
   </si>
   <si>
-    <t>created_by</t>
-  </si>
-  <si>
-    <t>updated_by</t>
+    <t>created_by_id</t>
+  </si>
+  <si>
+    <t>updated_by_id</t>
   </si>
   <si>
     <t>title</t>
@@ -159,6 +159,9 @@
     <t>actual_end_date</t>
   </si>
   <si>
+    <t>is_done</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -174,10 +177,10 @@
     <t>id_message</t>
   </si>
   <si>
-    <t xml:space="preserve">user_id (from)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_id (to)</t>
+    <t>from_user_id</t>
+  </si>
+  <si>
+    <t>to_user_id</t>
   </si>
   <si>
     <t>content_attachment</t>
@@ -186,19 +189,19 @@
     <t>message_task</t>
   </si>
   <si>
-    <t xml:space="preserve">id_task (to)</t>
+    <t>to_id_task</t>
   </si>
   <si>
     <t>message_group</t>
   </si>
   <si>
-    <t xml:space="preserve">id_group (to)</t>
+    <t>to_id_group</t>
   </si>
   <si>
     <t>message_sub_group</t>
   </si>
   <si>
-    <t xml:space="preserve">id_sub_group (to)</t>
+    <t>to_id_sub_group</t>
   </si>
 </sst>
 </file>
@@ -272,23 +275,29 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +812,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="I2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -826,7 +835,7 @@
     <col customWidth="1" min="16" max="16" width="13.140625"/>
     <col customWidth="1" min="17" max="17" width="12.28125"/>
     <col customWidth="1" min="18" max="18" width="14.57421875"/>
-    <col customWidth="1" min="19" max="19" width="12.28125"/>
+    <col customWidth="1" min="19" max="19" width="14.7109375"/>
     <col customWidth="1" min="20" max="20" width="12.00390625"/>
     <col customWidth="1" min="21" max="21" width="15.8515625"/>
     <col customWidth="1" min="22" max="22" width="13.140625"/>
@@ -849,7 +858,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="1"/>
@@ -863,124 +872,124 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9">
         <v>0</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="K6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" s="7" t="b">
+      <c r="O6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="V6" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" ht="14.25"/>
     <row r="10" ht="14.25">
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N10" s="1"/>
@@ -996,140 +1005,140 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="Q11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="R11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="T11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="U11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V11" s="3" t="s">
+      <c r="V11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="W11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="X11" s="3" t="s">
+      <c r="X11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="9">
         <v>0</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="9">
         <v>0</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="S12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="W12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="X12" s="8" t="b">
+      <c r="Q12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="V12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" s="11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7" t="s">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="8" t="b">
+      <c r="Q13" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="R13" s="8" t="b">
+      <c r="R13" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="S13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="V13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="W13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="X13" s="8" t="b">
+      <c r="S13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="V13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X13" s="11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="17" ht="14.25"/>
     <row r="18" ht="14.25">
@@ -1146,29 +1155,33 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" ht="14.25"/>
+    <row r="20" ht="14.25">
+      <c r="B20" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25"/>
     <row r="23" ht="14.25">
@@ -1188,59 +1201,63 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="N24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="P24" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1254,68 +1271,73 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="B29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="N29" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="O29" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
     </row>
     <row r="33" ht="14.25">
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1323,34 +1345,34 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="B34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="D34" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="E34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="B38" s="1" t="s">
-        <v>55</v>
+      <c r="B38" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1358,35 +1380,35 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>54</v>
+      <c r="C39" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="42" ht="14.25"/>
     <row r="43" ht="14.25">
-      <c r="B43" s="1" t="s">
-        <v>57</v>
+      <c r="B43" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1394,35 +1416,35 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" ht="14.25">
-      <c r="B44" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>54</v>
+      <c r="C44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="47" ht="14.25"/>
     <row r="48" ht="14.25">
-      <c r="B48" s="1" t="s">
-        <v>59</v>
+      <c r="B48" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1430,30 +1452,30 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="B49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>54</v>
+      <c r="C49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1463,8 +1485,8 @@
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B23:O23"/>
-    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B28:O28"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B38:F38"/>
     <mergeCell ref="B43:F43"/>

</xml_diff>